<commit_message>
final changes in project
</commit_message>
<xml_diff>
--- a/7rMartProject/src/test/resources/TestData.xlsx
+++ b/7rMartProject/src/test/resources/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16035" windowHeight="6060" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="LoginPage" sheetId="1" r:id="rId1"/>
@@ -12,12 +12,13 @@
     <sheet name="ManageNewsPage" sheetId="6" r:id="rId3"/>
     <sheet name="AdminUsersPage" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1:N18"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="14">
   <si>
     <t>UsernamePassword</t>
   </si>
@@ -56,6 +57,9 @@
   </si>
   <si>
     <t>watch</t>
+  </si>
+  <si>
+    <t>Staff</t>
   </si>
 </sst>
 </file>
@@ -461,7 +465,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -521,10 +525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B2"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -549,6 +553,11 @@
         <v>11</v>
       </c>
     </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>